<commit_message>
Fixed up course view per 5/3 meeting, added EE106 to bulk populator
</commit_message>
<xml_diff>
--- a/MDFDatabase/MDFDatabase/models/MDFS.xlsx
+++ b/MDFDatabase/MDFDatabase/models/MDFS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MDFDatabase\MDFDatabaseApp\mdf_db_app\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwb14182\Documents\MDFDatabase\MDFDatabase\MDFDatabase\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E92185-DFC8-48E6-A277-7EC3BDB0D4F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="451">
   <si>
     <t>Code</t>
   </si>
@@ -2978,11 +2979,138 @@
   <si>
     <t>EE467, EE311</t>
   </si>
+  <si>
+    <t>EE106</t>
+  </si>
+  <si>
+    <t>Electronic Design For Software
+Development 1</t>
+  </si>
+  <si>
+    <t>This module will provide an introduction to the practice of computer programming. It is assumed troughout that</t>
+  </si>
+  <si>
+    <t>the students have no prior exposure to programming.</t>
+  </si>
+  <si>
+    <t>The course begins with an introduction to data types and their associated operators, before examinging basic</t>
+  </si>
+  <si>
+    <t>flow control in the form of decisions (if-else) and iteration (for/while loops). Problem decomposition through</t>
+  </si>
+  <si>
+    <t>functions is discussed. Bespoke data types are addressed, and finally object oriented design principles are</t>
+  </si>
+  <si>
+    <t>taught (inheritance and polymorphism).</t>
+  </si>
+  <si>
+    <t>The first semester is based upon small self-contained problem sets to encourange problem solving skills while</t>
+  </si>
+  <si>
+    <t>cementing core concepts. The second semester involves small focussed projects undertaken in pairs.</t>
+  </si>
+  <si>
+    <t>The programming language used in this module is Python; this permits the programmer to concentrate on the</t>
+  </si>
+  <si>
+    <t>problem solving aspects and core techniques of programming rather than being distracted by the syntax of the</t>
+  </si>
+  <si>
+    <t>language.</t>
+  </si>
+  <si>
+    <t>functional decomposition.</t>
+  </si>
+  <si>
+    <t>LO 1: To demonstrate a deep understanding of primitive data types, then later abstract data types.</t>
+  </si>
+  <si>
+    <t>LO 2: To demonstrate a deep understanding of basic programming constructions: if-else, for, while etc.</t>
+  </si>
+  <si>
+    <t>LO 3: To develop an understanding of systematic problem solving via the divide-and-conquer approach of</t>
+  </si>
+  <si>
+    <t>LO 4: To develop self-reliance on programming by finding solutions to problems on own initiative.</t>
+  </si>
+  <si>
+    <t>LO 5: To learn to document code and produce software reports</t>
+  </si>
+  <si>
+    <t>This module will begin by teaching how to use the in-built Python GUI (IDLE) and interpretor.</t>
+  </si>
+  <si>
+    <t>The analogy of a computer program to a cooking recipe is used teach the dsitinction between data types and</t>
+  </si>
+  <si>
+    <t>algorithms.</t>
+  </si>
+  <si>
+    <t>The first semester is run as taught course in 3 main subsections: Data Types &amp; Operators, Algorithmic</t>
+  </si>
+  <si>
+    <t>Components (if-else, for, while, etc.), and program structure (functions, objects). In this semester, various</t>
+  </si>
+  <si>
+    <t>problem sets on these concepts are provided.</t>
+  </si>
+  <si>
+    <t>The second semester is run as a programming project section. Groups of 2 are assigned a topic that is to be</t>
+  </si>
+  <si>
+    <t>completed over a 10 week period. The emphasis in this semester is on problem solving and self-reliance.</t>
+  </si>
+  <si>
+    <t>LO1</t>
+  </si>
+  <si>
+    <t>LO2</t>
+  </si>
+  <si>
+    <t>LO3</t>
+  </si>
+  <si>
+    <t>LO4</t>
+  </si>
+  <si>
+    <t>C 1: Progression through work sets</t>
+  </si>
+  <si>
+    <t>C 2: Semester 1 multiple choice exam</t>
+  </si>
+  <si>
+    <t>C 2: Semester 1 exam</t>
+  </si>
+  <si>
+    <t>C 1: Second semester software design project: interim report, final report, demonstration</t>
+  </si>
+  <si>
+    <t>Students are provided with a score at the end of a multiple choice exam at the end of semester 1. Feedback is</t>
+  </si>
+  <si>
+    <t>also provided after assessment of an interim report on week 5 of semester 2.</t>
+  </si>
+  <si>
+    <t>Overall average is calculated as follows: Demonstrated Exercises (30%), Semester 1 test (10%), Interim Report</t>
+  </si>
+  <si>
+    <t>(20%), Final Report (20%), Demonstraion (20%).</t>
+  </si>
+  <si>
+    <t>Dive into Python 3. Other free material available online.</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3115,28 +3243,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S1048576" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A1:S1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:S1048576" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A1:S1048576" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="Code" dataDxfId="18"/>
-    <tableColumn id="2" name="Name" dataDxfId="17"/>
-    <tableColumn id="3" name="Credits" dataDxfId="16"/>
-    <tableColumn id="4" name="Semester" dataDxfId="15"/>
-    <tableColumn id="5" name="Elective" dataDxfId="14"/>
-    <tableColumn id="6" name="Level" dataDxfId="13"/>
-    <tableColumn id="7" name="Aims" dataDxfId="12"/>
-    <tableColumn id="8" name="Los" dataDxfId="11"/>
-    <tableColumn id="9" name="Syllabus" dataDxfId="10"/>
-    <tableColumn id="10" name="Criteria" dataDxfId="9"/>
-    <tableColumn id="11" name="Feedback" dataDxfId="8"/>
-    <tableColumn id="12" name="Comments" dataDxfId="7"/>
-    <tableColumn id="13" name="Reading" dataDxfId="6"/>
-    <tableColumn id="14" name="Reqs" dataDxfId="5"/>
-    <tableColumn id="15" name="lec" dataDxfId="4"/>
-    <tableColumn id="16" name="tut" dataDxfId="3"/>
-    <tableColumn id="17" name="ass" dataDxfId="2"/>
-    <tableColumn id="18" name="lab" dataDxfId="1"/>
-    <tableColumn id="19" name="study" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Code" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Credits" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Semester" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Elective" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Level" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Aims" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Los" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Syllabus" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Criteria" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Feedback" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Comments" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Reading" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Reqs" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="lec" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="tut" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ass" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="lab" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="study" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3404,11 +3532,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5702,7 +5830,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>400</v>
       </c>
@@ -5750,6 +5878,181 @@
       </c>
       <c r="S42" s="1" t="s">
         <v>407</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G44" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G45" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G46" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G47" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G48" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G49" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G50" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G51" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G52" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G53" s="1" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>